<commit_message>
update models and data
</commit_message>
<xml_diff>
--- a/OsimModelInfo/Uhlrich2022_info.xlsx
+++ b/OsimModelInfo/Uhlrich2022_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_data\Muscle_parameter_fitting\Replication\OsimModelInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDD43F0-EAA9-4552-B960-4A72B87549ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3F1374-05CA-4C33-8D63-C73709BEC84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1035" windowWidth="29040" windowHeight="17640" xr2:uid="{C026CD53-FE91-4BAC-A781-C7FFFE2D91BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C026CD53-FE91-4BAC-A781-C7FFFE2D91BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Muscles" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="58">
   <si>
     <t>HipKnee</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>addmagMid</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>piri</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186FB09B-09CF-4B9A-BB8A-055DD400A0EE}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U16:U17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +577,7 @@
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,8 +593,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -604,8 +613,11 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -621,8 +633,11 @@
       <c r="E3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -635,8 +650,11 @@
       <c r="E4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -649,8 +667,11 @@
       <c r="E5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -660,71 +681,208 @@
       <c r="E6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -734,15 +892,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F589C79C-BBF6-46EA-A053-C9ACA3C21E69}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,8 +916,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -775,8 +936,11 @@
       <c r="E2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -789,8 +953,11 @@
       <c r="E3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -800,10 +967,26 @@
       <c r="D4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -813,15 +996,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D31791A-354D-4709-B9E1-9512D998E745}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -837,8 +1020,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -854,8 +1040,11 @@
       <c r="E2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -871,8 +1060,11 @@
       <c r="E3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -882,18 +1074,32 @@
       <c r="D4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -903,15 +1109,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CCED9D-7013-409C-AFE5-E34CAEF36633}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,8 +1133,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -944,8 +1153,11 @@
       <c r="E2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -959,6 +1171,19 @@
         <v>48</v>
       </c>
       <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>